<commit_message>
plant database and parallelism
</commit_message>
<xml_diff>
--- a/test/2_REnamed_MS_experiment.xlsx
+++ b/test/2_REnamed_MS_experiment.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP135"/>
+  <dimension ref="A1:AP132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6764,8 +6764,10 @@
       <c r="A75" t="n">
         <v>387.3272</v>
       </c>
-      <c r="B75" t="n">
-        <v>39748</v>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>39748 // 39749</t>
+        </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -6842,10 +6844,8 @@
       <c r="A76" t="n">
         <v>387.3272</v>
       </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>39749 // 40342</t>
-        </is>
+      <c r="B76" t="n">
+        <v>40342</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -6882,21 +6882,21 @@
       <c r="S76" t="inlineStr"/>
       <c r="T76" t="inlineStr">
         <is>
-          <t>LMST03020075</t>
+          <t>LMST03020679</t>
         </is>
       </c>
       <c r="U76" t="n">
-        <v>42015</v>
+        <v>42605</v>
       </c>
       <c r="V76" t="inlineStr"/>
       <c r="W76" t="inlineStr">
         <is>
-          <t>PDCWVQZLMVLGLG-SDPFTLJPSA-N</t>
+          <t>PDCWVQZLMVLGLG-YQRSRUBMSA-N</t>
         </is>
       </c>
       <c r="X76" t="inlineStr">
         <is>
-          <t>CC(C)(O)CCC[C@@H](C)[C@H]1CC[C@H]2/C(/CCC[C@]12C)=C/C=C(/CCO)\C(=C)CO</t>
+          <t>CC(C)(O)CCC[C@@H](C)[C@H]1CC[C@H]2/C(/CCC[C@]12C)=C/C=C(\CCO)/C(=C)CO</t>
         </is>
       </c>
       <c r="Y76" t="inlineStr"/>
@@ -11210,8 +11210,10 @@
       <c r="A129" t="n">
         <v>603.5365</v>
       </c>
-      <c r="B129" t="n">
-        <v>31306</v>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>31306 // 31307</t>
+        </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
@@ -11226,7 +11228,7 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Behenyl myristoleate</t>
+          <t>Myristoleyl behenate</t>
         </is>
       </c>
       <c r="G129" t="inlineStr"/>
@@ -11288,8 +11290,10 @@
       <c r="A130" t="n">
         <v>603.5365</v>
       </c>
-      <c r="B130" t="n">
-        <v>31307</v>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>31308 // 31310</t>
+        </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
@@ -11304,7 +11308,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Myristoleyl behenate</t>
+          <t>Stearyl oleate</t>
         </is>
       </c>
       <c r="G130" t="inlineStr"/>
@@ -11326,21 +11330,21 @@
       <c r="S130" t="inlineStr"/>
       <c r="T130" t="inlineStr">
         <is>
-          <t>LMFA07010156</t>
+          <t>LMFA07010157</t>
         </is>
       </c>
       <c r="U130" t="n">
-        <v>97142</v>
+        <v>97143</v>
       </c>
       <c r="V130" t="inlineStr"/>
       <c r="W130" t="inlineStr">
         <is>
-          <t>GDAMRTVPVKYFCC-BENRWUELSA-N</t>
+          <t>YYDZACXIVKPEAI-ZPHPHTNESA-N</t>
         </is>
       </c>
       <c r="X130" t="inlineStr">
         <is>
-          <t>O=C(CCCCCCCCCCCCCCCCCCCCC)OCCCCCCCC/C=CCCCC</t>
+          <t>O=C(CCCCCCCCCCCCCCCCC)OCCCCCCCC/C=CCCCCCCCC</t>
         </is>
       </c>
       <c r="Y130" t="inlineStr"/>
@@ -11366,8 +11370,10 @@
       <c r="A131" t="n">
         <v>603.5365</v>
       </c>
-      <c r="B131" t="n">
-        <v>31308</v>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>31309 // 31175</t>
+        </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
@@ -11382,7 +11388,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Oleyl stearate</t>
+          <t>Arachidyl palmitoleate</t>
         </is>
       </c>
       <c r="G131" t="inlineStr"/>
@@ -11404,21 +11410,21 @@
       <c r="S131" t="inlineStr"/>
       <c r="T131" t="inlineStr">
         <is>
-          <t>LMFA07010157</t>
+          <t>LMFA07010158</t>
         </is>
       </c>
       <c r="U131" t="n">
-        <v>97143</v>
+        <v>97144</v>
       </c>
       <c r="V131" t="inlineStr"/>
       <c r="W131" t="inlineStr">
         <is>
-          <t>YYDZACXIVKPEAI-ZPHPHTNESA-N</t>
+          <t>IKZAMBGSRXDRMP-PEZBUJJGSA-N</t>
         </is>
       </c>
       <c r="X131" t="inlineStr">
         <is>
-          <t>O=C(CCCCCCCCCCCCCCCCC)OCCCCCCCC/C=CCCCCCCCC</t>
+          <t>O=C(CCCCCCCCCCCCCCCCCCC)OCCCCCCCC/C=CCCCCCC</t>
         </is>
       </c>
       <c r="Y131" t="inlineStr"/>
@@ -11445,7 +11451,7 @@
         <v>603.5365</v>
       </c>
       <c r="B132" t="n">
-        <v>31309</v>
+        <v>31156</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
@@ -11460,7 +11466,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>Palmitoleyl arachidate</t>
+          <t>octadecenyl heptadecanoate</t>
         </is>
       </c>
       <c r="G132" t="inlineStr"/>
@@ -11482,21 +11488,21 @@
       <c r="S132" t="inlineStr"/>
       <c r="T132" t="inlineStr">
         <is>
-          <t>LMFA07010158</t>
+          <t>LMFA07010005</t>
         </is>
       </c>
       <c r="U132" t="n">
-        <v>97144</v>
+        <v>46539</v>
       </c>
       <c r="V132" t="inlineStr"/>
       <c r="W132" t="inlineStr">
         <is>
-          <t>IKZAMBGSRXDRMP-PEZBUJJGSA-N</t>
+          <t>CWCJUHWQOPRDLE-QZQOTICOSA-N</t>
         </is>
       </c>
       <c r="X132" t="inlineStr">
         <is>
-          <t>O=C(CCCCCCCCCCCCCCCCCCC)OCCCCCCCC/C=CCCCCCC</t>
+          <t>C(C)CCCCCCCCCCCCCCC(OCCCCCCC/C=C/CCCCCCCCCC)=O</t>
         </is>
       </c>
       <c r="Y132" t="inlineStr"/>
@@ -11518,240 +11524,6 @@
       <c r="AO132" t="inlineStr"/>
       <c r="AP132" t="inlineStr"/>
     </row>
-    <row r="133">
-      <c r="A133" t="n">
-        <v>603.5365</v>
-      </c>
-      <c r="B133" t="n">
-        <v>31310</v>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>M+H+HCOONa</t>
-        </is>
-      </c>
-      <c r="D133" t="n">
-        <v>8</v>
-      </c>
-      <c r="E133" t="n">
-        <v>534.5376</v>
-      </c>
-      <c r="F133" t="inlineStr">
-        <is>
-          <t>Stearyl oleate</t>
-        </is>
-      </c>
-      <c r="G133" t="inlineStr"/>
-      <c r="H133" t="inlineStr"/>
-      <c r="I133" t="inlineStr"/>
-      <c r="J133" t="inlineStr"/>
-      <c r="K133" t="inlineStr"/>
-      <c r="L133" t="inlineStr">
-        <is>
-          <t>C36H70O2</t>
-        </is>
-      </c>
-      <c r="M133" t="inlineStr"/>
-      <c r="N133" t="inlineStr"/>
-      <c r="O133" t="inlineStr"/>
-      <c r="P133" t="inlineStr"/>
-      <c r="Q133" t="inlineStr"/>
-      <c r="R133" t="inlineStr"/>
-      <c r="S133" t="inlineStr"/>
-      <c r="T133" t="inlineStr">
-        <is>
-          <t>LMFA07010159</t>
-        </is>
-      </c>
-      <c r="U133" t="n">
-        <v>97145</v>
-      </c>
-      <c r="V133" t="inlineStr"/>
-      <c r="W133" t="inlineStr">
-        <is>
-          <t>WRPMUZXHQKAAIC-ZZEZOPTASA-N</t>
-        </is>
-      </c>
-      <c r="X133" t="inlineStr">
-        <is>
-          <t>O=C(CCCCCCC/C=CCCCCCCCC)OCCCCCCCCCCCCCCCCCC</t>
-        </is>
-      </c>
-      <c r="Y133" t="inlineStr"/>
-      <c r="Z133" t="inlineStr"/>
-      <c r="AA133" t="inlineStr"/>
-      <c r="AB133" t="inlineStr"/>
-      <c r="AC133" t="inlineStr"/>
-      <c r="AD133" t="inlineStr"/>
-      <c r="AE133" t="inlineStr"/>
-      <c r="AF133" t="inlineStr"/>
-      <c r="AG133" t="inlineStr"/>
-      <c r="AH133" t="inlineStr"/>
-      <c r="AI133" t="inlineStr"/>
-      <c r="AJ133" t="inlineStr"/>
-      <c r="AK133" t="inlineStr"/>
-      <c r="AL133" t="inlineStr"/>
-      <c r="AM133" t="inlineStr"/>
-      <c r="AN133" t="inlineStr"/>
-      <c r="AO133" t="inlineStr"/>
-      <c r="AP133" t="inlineStr"/>
-    </row>
-    <row r="134">
-      <c r="A134" t="n">
-        <v>603.5365</v>
-      </c>
-      <c r="B134" t="n">
-        <v>31156</v>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>M+H+HCOONa</t>
-        </is>
-      </c>
-      <c r="D134" t="n">
-        <v>8</v>
-      </c>
-      <c r="E134" t="n">
-        <v>534.5376</v>
-      </c>
-      <c r="F134" t="inlineStr">
-        <is>
-          <t>octadecenyl heptadecanoate</t>
-        </is>
-      </c>
-      <c r="G134" t="inlineStr"/>
-      <c r="H134" t="inlineStr"/>
-      <c r="I134" t="inlineStr"/>
-      <c r="J134" t="inlineStr"/>
-      <c r="K134" t="inlineStr"/>
-      <c r="L134" t="inlineStr">
-        <is>
-          <t>C36H70O2</t>
-        </is>
-      </c>
-      <c r="M134" t="inlineStr"/>
-      <c r="N134" t="inlineStr"/>
-      <c r="O134" t="inlineStr"/>
-      <c r="P134" t="inlineStr"/>
-      <c r="Q134" t="inlineStr"/>
-      <c r="R134" t="inlineStr"/>
-      <c r="S134" t="inlineStr"/>
-      <c r="T134" t="inlineStr">
-        <is>
-          <t>LMFA07010005</t>
-        </is>
-      </c>
-      <c r="U134" t="n">
-        <v>46539</v>
-      </c>
-      <c r="V134" t="inlineStr"/>
-      <c r="W134" t="inlineStr">
-        <is>
-          <t>CWCJUHWQOPRDLE-QZQOTICOSA-N</t>
-        </is>
-      </c>
-      <c r="X134" t="inlineStr">
-        <is>
-          <t>C(C)CCCCCCCCCCCCCCC(OCCCCCCC/C=C/CCCCCCCCCC)=O</t>
-        </is>
-      </c>
-      <c r="Y134" t="inlineStr"/>
-      <c r="Z134" t="inlineStr"/>
-      <c r="AA134" t="inlineStr"/>
-      <c r="AB134" t="inlineStr"/>
-      <c r="AC134" t="inlineStr"/>
-      <c r="AD134" t="inlineStr"/>
-      <c r="AE134" t="inlineStr"/>
-      <c r="AF134" t="inlineStr"/>
-      <c r="AG134" t="inlineStr"/>
-      <c r="AH134" t="inlineStr"/>
-      <c r="AI134" t="inlineStr"/>
-      <c r="AJ134" t="inlineStr"/>
-      <c r="AK134" t="inlineStr"/>
-      <c r="AL134" t="inlineStr"/>
-      <c r="AM134" t="inlineStr"/>
-      <c r="AN134" t="inlineStr"/>
-      <c r="AO134" t="inlineStr"/>
-      <c r="AP134" t="inlineStr"/>
-    </row>
-    <row r="135">
-      <c r="A135" t="n">
-        <v>603.5365</v>
-      </c>
-      <c r="B135" t="n">
-        <v>31175</v>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>M+H+HCOONa</t>
-        </is>
-      </c>
-      <c r="D135" t="n">
-        <v>8</v>
-      </c>
-      <c r="E135" t="n">
-        <v>534.5376</v>
-      </c>
-      <c r="F135" t="inlineStr">
-        <is>
-          <t>Arachidyl palmitoleate</t>
-        </is>
-      </c>
-      <c r="G135" t="inlineStr"/>
-      <c r="H135" t="inlineStr"/>
-      <c r="I135" t="inlineStr"/>
-      <c r="J135" t="inlineStr"/>
-      <c r="K135" t="inlineStr"/>
-      <c r="L135" t="inlineStr">
-        <is>
-          <t>C36H70O2</t>
-        </is>
-      </c>
-      <c r="M135" t="inlineStr"/>
-      <c r="N135" t="inlineStr"/>
-      <c r="O135" t="inlineStr"/>
-      <c r="P135" t="inlineStr"/>
-      <c r="Q135" t="inlineStr"/>
-      <c r="R135" t="inlineStr"/>
-      <c r="S135" t="inlineStr"/>
-      <c r="T135" t="inlineStr">
-        <is>
-          <t>LMFA07010024</t>
-        </is>
-      </c>
-      <c r="U135" t="n">
-        <v>75403</v>
-      </c>
-      <c r="V135" t="inlineStr"/>
-      <c r="W135" t="inlineStr">
-        <is>
-          <t>FIETWBRPSYJUOM-PEZBUJJGSA-N</t>
-        </is>
-      </c>
-      <c r="X135" t="inlineStr">
-        <is>
-          <t>O=C(CCCCCCC/C=CCCCCCC)OCCCCCCCCCCCCCCCCCCCC</t>
-        </is>
-      </c>
-      <c r="Y135" t="inlineStr"/>
-      <c r="Z135" t="inlineStr"/>
-      <c r="AA135" t="inlineStr"/>
-      <c r="AB135" t="inlineStr"/>
-      <c r="AC135" t="inlineStr"/>
-      <c r="AD135" t="inlineStr"/>
-      <c r="AE135" t="inlineStr"/>
-      <c r="AF135" t="inlineStr"/>
-      <c r="AG135" t="inlineStr"/>
-      <c r="AH135" t="inlineStr"/>
-      <c r="AI135" t="inlineStr"/>
-      <c r="AJ135" t="inlineStr"/>
-      <c r="AK135" t="inlineStr"/>
-      <c r="AL135" t="inlineStr"/>
-      <c r="AM135" t="inlineStr"/>
-      <c r="AN135" t="inlineStr"/>
-      <c r="AO135" t="inlineStr"/>
-      <c r="AP135" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>